<commit_message>
- dodano opis danych dodatkowych - zmodyfikowano chunk z dodatkowymi kolumnami - usunieto kategorie wieku mieszkan - zmodyfikowano kod wykresow boxplot z 3x3 na 3x3 na jedna strone i 2x3 na druga - dodano opis i interpretacje wykresow boxplot
</commit_message>
<xml_diff>
--- a/Zadania.xlsx
+++ b/Zadania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C33F762-F21F-4B20-9C2F-EF3EEC8EEEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C70D81A-1804-4170-92A7-05EDF153CC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To_Do" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <r>
       <t>Sprawdzenie spójności danych</t>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>Zweryfikować logiczną spójność wartości, np. sprawdzić, czy piętro nie przekracza całkowitej liczby kondygnacji, rok budowy nie jest późniejszy niż bieżący rok, a liczba pokoi nie jest ujemna lub zerowa: za pomocą library(validate)</t>
+  </si>
+  <si>
+    <t>Komentarz</t>
+  </si>
+  <si>
+    <t>Usunięte - pokrywa się z punktem 4 w Hipotezach (rok budowy)</t>
+  </si>
+  <si>
+    <t>Zmiana nazwy chunk, usunięcie kategorii wieku mieszkania.</t>
+  </si>
+  <si>
+    <t>Sprawdzić z dziewczynami na spotkaniu</t>
   </si>
 </sst>
 </file>
@@ -322,7 +334,10 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -354,13 +369,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -435,14 +450,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CAF075B-1E8A-4A21-A700-F2276D89C34D}" name="Tabela1" displayName="Tabela1" ref="A1:E36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
-  <autoFilter ref="A1:E36" xr:uid="{9CAF075B-1E8A-4A21-A700-F2276D89C34D}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A0752BE9-2E16-4D4A-BF52-D2AB4C4AC727}" name="Numer" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{333BDF78-DAC8-496E-90BB-8077CFED2086}" name="Opis" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4BC94FA0-9C0C-41D0-BF83-0F6A9FC9F584}" name="Osoba" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00735EEA-43B5-49C3-8B2E-7B2F3F58CD58}" name="Do kiedy?" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{5B1A65D0-D223-4C13-AA2E-03CDDDEA8A34}" name="Status" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CAF075B-1E8A-4A21-A700-F2276D89C34D}" name="Tabela1" displayName="Tabela1" ref="A1:F36" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:F36" xr:uid="{9CAF075B-1E8A-4A21-A700-F2276D89C34D}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A0752BE9-2E16-4D4A-BF52-D2AB4C4AC727}" name="Numer" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{333BDF78-DAC8-496E-90BB-8077CFED2086}" name="Opis" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{4BC94FA0-9C0C-41D0-BF83-0F6A9FC9F584}" name="Osoba" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00735EEA-43B5-49C3-8B2E-7B2F3F58CD58}" name="Do kiedy?" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{5B1A65D0-D223-4C13-AA2E-03CDDDEA8A34}" name="Status" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{4E76C389-1B5D-46CC-BE52-1FD6E2F8EF8A}" name="Komentarz" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -717,7 +733,7 @@
   <dimension ref="A1:N437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,6 +743,7 @@
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="58.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -745,6 +762,9 @@
       <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -760,6 +780,7 @@
         <v>45644</v>
       </c>
       <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
@@ -777,7 +798,12 @@
       <c r="D3" s="6">
         <v>45644</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="N3" s="3" t="s">
         <v>14</v>
       </c>
@@ -795,7 +821,10 @@
       <c r="D4" s="6">
         <v>45644</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="N4" s="3" t="s">
         <v>15</v>
       </c>
@@ -813,7 +842,12 @@
       <c r="D5" s="6">
         <v>45644</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -829,6 +863,7 @@
         <v>45644</v>
       </c>
       <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -844,6 +879,7 @@
         <v>45644</v>
       </c>
       <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -859,6 +895,7 @@
         <v>45644</v>
       </c>
       <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -874,6 +911,7 @@
         <v>45644</v>
       </c>
       <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -889,6 +927,7 @@
         <v>45644</v>
       </c>
       <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -903,7 +942,12 @@
       <c r="D11" s="6">
         <v>45644</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -913,6 +957,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -922,6 +967,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="N13" s="3" t="s">
         <v>17</v>
       </c>
@@ -934,6 +980,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="N14" s="3" t="s">
         <v>18</v>
       </c>
@@ -946,6 +993,7 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="N15" s="3" t="s">
         <v>19</v>
       </c>
@@ -958,6 +1006,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="N16" s="3" t="s">
         <v>20</v>
       </c>
@@ -970,6 +1019,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="N17" s="3" t="s">
         <v>21</v>
       </c>
@@ -982,6 +1032,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="N18" s="3" t="s">
         <v>22</v>
       </c>
@@ -994,6 +1045,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -1003,6 +1055,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -1012,6 +1065,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1021,6 +1075,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -1030,6 +1085,7 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
@@ -1039,6 +1095,7 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -1048,6 +1105,7 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
@@ -1057,6 +1115,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -1066,6 +1125,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
@@ -1075,6 +1135,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
@@ -1084,6 +1145,7 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
@@ -1093,6 +1155,7 @@
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
@@ -1102,6 +1165,7 @@
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
@@ -1111,8 +1175,9 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1120,8 +1185,9 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1129,8 +1195,9 @@
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1138,8 +1205,9 @@
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1147,74 +1215,75 @@
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="4"/>
@@ -3556,13 +3625,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C623">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Piotr"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Klaudia"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Iza"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- zespolowy przeglad zadan - aktualizacja statusow - wyznaczenie nowych zadan
</commit_message>
<xml_diff>
--- a/Zadania.xlsx
+++ b/Zadania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C70D81A-1804-4170-92A7-05EDF153CC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787ED128-71B7-4A1A-B9E3-D7D37E77796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1500" windowWidth="27825" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To_Do" sheetId="1" r:id="rId1"/>
@@ -88,12 +88,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{8B5F0258-3759-4AA5-A2C5-26971FF4B63D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">Podział walidacji na 2 części - wstępna przed wranglingiem
+Druga - w celu sprawdzenia wyniku z data wrangling
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <r>
       <t>Sprawdzenie spójności danych</t>
@@ -246,6 +262,27 @@
   </si>
   <si>
     <t>Sprawdzić z dziewczynami na spotkaniu</t>
+  </si>
+  <si>
+    <t>Test Grubbsa - usunięty. Zastąpiony testem Z-score i skośnością.</t>
+  </si>
+  <si>
+    <t>Refki do wykresów box-plot. Przeniesienie do wykresu z opisu</t>
+  </si>
+  <si>
+    <t>Weryfikacja wielkosci nagłówków</t>
+  </si>
+  <si>
+    <t>Hist - dodanie rozkładu normalnego</t>
+  </si>
+  <si>
+    <t>Wstep, po co sprawdzamy, czym się charakteryzuja i wypisac jakie my mamy</t>
+  </si>
+  <si>
+    <t>Czemu to sprawdzamy. Jak to sprawdzamy, co nam to dało.</t>
+  </si>
+  <si>
+    <t>Hist - opisanie wykresow i rozkalu normalnego</t>
   </si>
 </sst>
 </file>
@@ -336,9 +373,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF9999FF"/>
@@ -358,6 +392,9 @@
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -458,7 +495,7 @@
     <tableColumn id="3" xr3:uid="{4BC94FA0-9C0C-41D0-BF83-0F6A9FC9F584}" name="Osoba" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{00735EEA-43B5-49C3-8B2E-7B2F3F58CD58}" name="Do kiedy?" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{5B1A65D0-D223-4C13-AA2E-03CDDDEA8A34}" name="Status" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{4E76C389-1B5D-46CC-BE52-1FD6E2F8EF8A}" name="Komentarz" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{4E76C389-1B5D-46CC-BE52-1FD6E2F8EF8A}" name="Komentarz" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -732,8 +769,8 @@
   </sheetPr>
   <dimension ref="A1:N437"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +780,7 @@
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -779,8 +816,12 @@
       <c r="D2" s="6">
         <v>45644</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
@@ -862,7 +903,9 @@
       <c r="D6" s="6">
         <v>45644</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -878,7 +921,9 @@
       <c r="D7" s="6">
         <v>45644</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -894,7 +939,9 @@
       <c r="D8" s="6">
         <v>45644</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -910,8 +957,12 @@
       <c r="D9" s="6">
         <v>45644</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -926,8 +977,12 @@
       <c r="D10" s="6">
         <v>45644</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -943,7 +998,7 @@
         <v>45644</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>38</v>
@@ -953,20 +1008,36 @@
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6">
+        <v>45644</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="6">
+        <v>45644</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="N13" s="3" t="s">
         <v>17</v>
@@ -976,10 +1047,18 @@
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="6">
+        <v>45644</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="N14" s="3" t="s">
         <v>18</v>
@@ -989,10 +1068,18 @@
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="6">
+        <v>45644</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="N15" s="3" t="s">
         <v>19</v>
@@ -3625,13 +3712,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C623">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Piotr"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Klaudia"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Iza"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- naprawa błędu skali w obserwacje_brakujace_wykresy_2 - naprawa zbyt wielu kombinacji w wykresie wzorce_brakow - interpretacja wyników histogramów - dodanie "kotwic" do przemieszczania się z opisu histogramu do wykresu w HTML - aktualizacja pliku zadania.xlsx + komentarze
</commit_message>
<xml_diff>
--- a/Zadania.xlsx
+++ b/Zadania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787ED128-71B7-4A1A-B9E3-D7D37E77796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D51608-B8A7-45E1-A6B0-B7CC10A7A2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1500" windowWidth="27825" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28650" yWindow="1620" windowWidth="27825" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To_Do" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <r>
       <t>Sprawdzenie spójności danych</t>
@@ -282,7 +282,10 @@
     <t>Czemu to sprawdzamy. Jak to sprawdzamy, co nam to dało.</t>
   </si>
   <si>
-    <t>Hist - opisanie wykresow i rozkalu normalnego</t>
+    <t>Hist - opisanie wykresow i rozkladu normalnego</t>
+  </si>
+  <si>
+    <t>Zrobione dla histogramów</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
   <dimension ref="A1:N437"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,9 +1021,11 @@
         <v>45644</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -1057,7 +1062,7 @@
         <v>45644</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F14" s="4"/>
       <c r="N14" s="3" t="s">
@@ -1078,7 +1083,7 @@
         <v>45644</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F15" s="4"/>
       <c r="N15" s="3" t="s">

</xml_diff>

<commit_message>
- aktualizacja statusu zadań
</commit_message>
<xml_diff>
--- a/Zadania.xlsx
+++ b/Zadania.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BDF415-DA41-466B-8EEB-401DDDBF515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9073F80-93E3-422F-BD6F-0C5871B63D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>Numer</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>Opis czym jest data wrangling</t>
+  </si>
+  <si>
+    <t>Brudne dane: czym są, na co wpływają</t>
   </si>
 </sst>
 </file>
@@ -1841,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N437"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2453,8 +2456,12 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="13"/>

</xml_diff>

<commit_message>
- aktualizacja i ustalenie kolejnych zadań
</commit_message>
<xml_diff>
--- a/Zadania.xlsx
+++ b/Zadania.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9073F80-93E3-422F-BD6F-0C5871B63D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A4D9AA-3296-4E42-B38F-4902A554FFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>Numer</t>
   </si>
@@ -328,6 +328,27 @@
   </si>
   <si>
     <t>Brudne dane: czym są, na co wpływają</t>
+  </si>
+  <si>
+    <t>walidacja_wstępna_danych - sprawdzić czy inny wykres będzie bardziej pasował shrek też do wymiany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walidacja kontrola danych - od wiersza 1067 </t>
+  </si>
+  <si>
+    <t>Woj.- dać punkty zamiast pogrubień nagłówków</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Udogodnienia - wykres typu boxplot </t>
+  </si>
+  <si>
+    <t>Interpretacja boxplot</t>
+  </si>
+  <si>
+    <t>Granice administracyjne dzielnic (Gdańsk, Warszawa, najtańsze)</t>
+  </si>
+  <si>
+    <t>Inwestycje - repo, word, przesłac link</t>
   </si>
 </sst>
 </file>
@@ -1844,9 +1865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N437"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2478,8 +2497,12 @@
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="15"/>
+      <c r="B24" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="13"/>
@@ -2496,8 +2519,12 @@
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
+      <c r="B25" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="13"/>
@@ -2514,8 +2541,12 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="15"/>
+      <c r="B26" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="13"/>
@@ -2532,8 +2563,12 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="15"/>
+      <c r="B27" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="13"/>
@@ -2550,8 +2585,12 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="15"/>
+      <c r="B28" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="13"/>
@@ -2568,8 +2607,12 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
+      <c r="B29" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="13"/>
@@ -2586,8 +2629,12 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="13"/>

</xml_diff>

<commit_message>
- Zaktualizowanie zadan - Dodanie 'Brudnych danych" - Aktualizacja wszystkich chunków po zmianie nazw kolumn - Opis zmian jakie naniesiono w ramach opisu brudnych danych - Dodanie kotwic do boxplotów - Usuniecie osi z wykresu sr. cen mieszkan - Zmiana szaty kolorystycznej sr. cen mieszkan - Zmiana punktow z interpretacja wynikow cen wojewodztw - dodanie danych geometrii dzielnic gdanska - dodanie opisu sylwetki gdanska - analiza i interpretacja cen mieszkan/m^2 w zaleznosci od dzielnicy
</commit_message>
<xml_diff>
--- a/Zadania.xlsx
+++ b/Zadania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A4D9AA-3296-4E42-B38F-4902A554FFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA42DEDC-D926-48F6-9540-82B9B172F97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To_Do" sheetId="2" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>Numer</t>
   </si>
@@ -350,6 +350,9 @@
   <si>
     <t>Inwestycje - repo, word, przesłac link</t>
   </si>
+  <si>
+    <t>Zrobiłem do Gdańska :)</t>
+  </si>
 </sst>
 </file>
 
@@ -556,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -623,6 +626,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2199,7 +2205,7 @@
         <v>45644</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>28</v>
@@ -2283,7 +2289,7 @@
         <v>45644</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="5"/>
@@ -2388,7 +2394,9 @@
       <c r="D19" s="10">
         <v>45646</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="F19" s="13"/>
       <c r="G19" s="5"/>
       <c r="H19" s="6"/>
@@ -2481,8 +2489,12 @@
       <c r="C23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="D23" s="10">
+        <v>45660</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="F23" s="13"/>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
@@ -2503,7 +2515,9 @@
       <c r="C24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="10">
+        <v>45660</v>
+      </c>
       <c r="E24" s="15"/>
       <c r="F24" s="13"/>
       <c r="G24" s="5"/>
@@ -2525,7 +2539,9 @@
       <c r="C25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="15"/>
+      <c r="D25" s="10">
+        <v>45660</v>
+      </c>
       <c r="E25" s="15"/>
       <c r="F25" s="13"/>
       <c r="G25" s="5"/>
@@ -2547,8 +2563,12 @@
       <c r="C26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="D26" s="10">
+        <v>45660</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="F26" s="13"/>
       <c r="G26" s="5"/>
       <c r="H26" s="6"/>
@@ -2569,7 +2589,9 @@
       <c r="C27" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="15"/>
+      <c r="D27" s="10">
+        <v>45660</v>
+      </c>
       <c r="E27" s="15"/>
       <c r="F27" s="13"/>
       <c r="G27" s="5"/>
@@ -2591,7 +2613,9 @@
       <c r="C28" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="15"/>
+      <c r="D28" s="10">
+        <v>45660</v>
+      </c>
       <c r="E28" s="15"/>
       <c r="F28" s="13"/>
       <c r="G28" s="5"/>
@@ -2613,9 +2637,15 @@
       <c r="C29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="13"/>
+      <c r="D29" s="10">
+        <v>45660</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>63</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -2635,8 +2665,12 @@
       <c r="C30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
+      <c r="D30" s="10">
+        <v>45646</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="F30" s="13"/>
       <c r="G30" s="5"/>
       <c r="H30" s="6"/>

</xml_diff>

<commit_message>
Dodanie opisu do drugiej walidacji - czemu ją wykonujemy, co nam to da
</commit_message>
<xml_diff>
--- a/Zadania.xlsx
+++ b/Zadania.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaudia\Desktop\projekty GIT\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE659137-9929-40D0-8A47-9CFFC1F7DEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Podsumowanie eksportu" sheetId="1" r:id="rId1"/>
@@ -23,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Oem</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
   <si>
     <t>Ten dokument został wyeksportowany z aplikacji Numbers. Każda z tabel została skonwertowana do arkusza aplikacji Excel. Pozostałe obiekty na każdym z arkuszy Numbers zostały umieszczone na osobnych arkuszach. Pamiętaj, że działanie formuł w aplikacji Excel może być inne.</t>
   </si>
@@ -402,7 +401,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -805,16 +804,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -945,7 +944,7 @@
         <xdr:cNvPr id="5" name="Obraz 1" descr="Obraz 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2053,7 +2052,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
@@ -2067,11 +2066,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="7" spans="2:4" ht="18.75">
       <c r="B7" s="1" t="s">
@@ -2137,20 +2136,20 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'To_Do'!R1C1" display="To_Do" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D12" location="'Notatki_11_12_24'!R1C1" display="Notatki_11_12_24" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D14" location="'Error_ScreenShots'!R1C1" display="Error_ScreenShots" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D10" location="'To_Do'!R1C1" display="To_Do"/>
+    <hyperlink ref="D12" location="'Notatki_11_12_24'!R1C1" display="Notatki_11_12_24"/>
+    <hyperlink ref="D14" location="'Error_ScreenShots'!R1C1" display="Error_ScreenShots"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N437"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2914,7 +2913,9 @@
       <c r="D28" s="14">
         <v>45660</v>
       </c>
-      <c r="E28" s="19"/>
+      <c r="E28" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="F28" s="17"/>
       <c r="G28" s="9"/>
       <c r="H28" s="10"/>
@@ -2983,7 +2984,7 @@
       <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="37" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="19"/>
@@ -3003,7 +3004,7 @@
       <c r="A32" s="11">
         <v>31</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="37" t="s">
         <v>74</v>
       </c>
       <c r="C32" s="19"/>
@@ -3023,7 +3024,7 @@
       <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="37" t="s">
         <v>75</v>
       </c>
       <c r="C33" s="19"/>
@@ -3043,7 +3044,7 @@
       <c r="A34" s="11">
         <v>33</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="37" t="s">
         <v>76</v>
       </c>
       <c r="C34" s="19"/>
@@ -3053,7 +3054,7 @@
       <c r="E34" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="38" t="s">
         <v>77</v>
       </c>
       <c r="G34" s="9"/>
@@ -3069,7 +3070,7 @@
       <c r="A35" s="11">
         <v>34</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="37" t="s">
         <v>78</v>
       </c>
       <c r="C35" s="19"/>
@@ -9532,10 +9533,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C437" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C437">
       <formula1>"Iza,Klaudia,Piotr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E318" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E318">
       <formula1>"Nowe,W trakcie,Blokowane/Wstrzymane,Do weryfikacji/Testowane,Zakończone,Anulowane"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9549,7 +9550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -9704,7 +9705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>

</xml_diff>